<commit_message>
lam xong danh muc ho so
</commit_message>
<xml_diff>
--- a/Assets/Excel/User/User.xlsx
+++ b/Assets/Excel/User/User.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B82BB-CF3C-48C0-9935-D0E399975881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC145C0-1E3E-444D-8330-04935C95DECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8532" yWindow="1212" windowWidth="14508" windowHeight="8964" xr2:uid="{4C36C905-F9B5-40D3-B57A-940CD66F6CDD}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{4C36C905-F9B5-40D3-B57A-940CD66F6CDD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>HoTen</t>
   </si>
@@ -92,6 +92,36 @@
   </si>
   <si>
     <t>qlnd</t>
+  </si>
+  <si>
+    <t>tài khoản 2</t>
+  </si>
+  <si>
+    <t>tài khoản 3</t>
+  </si>
+  <si>
+    <t>tài khoản 4</t>
+  </si>
+  <si>
+    <t>tài khoản 5</t>
+  </si>
+  <si>
+    <t>tài khoản 6</t>
+  </si>
+  <si>
+    <t>tài khoản 7</t>
+  </si>
+  <si>
+    <t>tài khoản 8</t>
+  </si>
+  <si>
+    <t>tài khoản 9</t>
+  </si>
+  <si>
+    <t>tài khoản 10</t>
+  </si>
+  <si>
+    <t>tài khoản 11</t>
   </si>
 </sst>
 </file>
@@ -101,10 +131,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +515,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,7 +593,7 @@
         <v>17</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>123123</v>
@@ -591,11 +627,17 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -607,7 +649,7 @@
         <v>18</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>123123</v>
@@ -616,7 +658,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -628,13 +670,13 @@
         <v>18</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -645,11 +687,14 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -660,11 +705,14 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -672,11 +720,14 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -684,11 +735,30 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -700,7 +770,7 @@
         <v>18</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>123123</v>
@@ -710,6 +780,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
thêm chức năng thêm hồ sơ bằng excel
</commit_message>
<xml_diff>
--- a/Assets/Excel/User/User.xlsx
+++ b/Assets/Excel/User/User.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teu-pc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DB020B-9964-4E42-AFAC-99A2862CD7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC814DB5-F1EE-440D-BE86-3DCC6F7BCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>HoTen</t>
   </si>
@@ -77,12 +77,6 @@
     <t>MaTrangThai</t>
   </si>
   <si>
-    <t>TenAnhDaiDien</t>
-  </si>
-  <si>
-    <t>DuongDan</t>
-  </si>
-  <si>
     <t>admin siêu đẹp trai</t>
   </si>
   <si>
@@ -95,12 +89,6 @@
     <t>Đóng</t>
   </si>
   <si>
-    <t>1545130_288016768030903_2199143617119502561_n.jpg</t>
-  </si>
-  <si>
-    <t>/Assets/Images/Avatars/User/1545130_288016768030903_2199143617119502561_n_637928409593639885.jpg</t>
-  </si>
-  <si>
     <t>quản lý người dùng</t>
   </si>
   <si>
@@ -113,24 +101,12 @@
     <t>Mở</t>
   </si>
   <si>
-    <t>1546135_288016861364227_1275175656542392177_n (1).jpg</t>
-  </si>
-  <si>
-    <t>/Assets/Images/Avatars/User/1546135_288016861364227_1275175656542392177_n (1)_637928409593659862.jpg</t>
-  </si>
-  <si>
     <t>quản lý knd</t>
   </si>
   <si>
     <t>qlknd</t>
   </si>
   <si>
-    <t>10401987_1609988362552899_7782344116794459612_n.jpg</t>
-  </si>
-  <si>
-    <t>/Assets/Images/Avatars/User/10401987_1609988362552899_7782344116794459612_n_637928409593659862.jpg</t>
-  </si>
-  <si>
     <t>vô danh tiểu tốt</t>
   </si>
   <si>
@@ -147,12 +123,6 @@
   </si>
   <si>
     <t>qldv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">khanh </t>
-  </si>
-  <si>
-    <t>ga</t>
   </si>
 </sst>
 </file>
@@ -194,7 +164,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -211,20 +206,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O2">
   <autoFilter ref="A1:O2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="HoTen"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="UserName"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Password"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="HoTen" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="UserName" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Password" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MaKieu"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TrangThai"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="SDT"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Email"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="NgaySinh"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="GioiTinh"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="DiaChi"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="QueQuan"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="CongTy"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="ChucVu"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="TieuSu"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="DiaChi" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="QueQuan" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="CongTy" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="ChucVu" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="TieuSu" dataDxfId="0"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="AnhDaiDien"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -259,17 +254,6 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TrangThai"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="MaTrangThai"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table5" displayName="Table5" ref="J1:K4">
-  <autoFilter ref="J1:K4" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TenAnhDaiDien"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DuongDan"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -575,7 +559,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,17 +628,17 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2">
-        <v>123</v>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -665,11 +649,26 @@
       <c r="G2">
         <v>123</v>
       </c>
+      <c r="H2" s="2">
+        <v>36558</v>
+      </c>
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>31</v>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -679,26 +678,20 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" xr:uid="{BD16BA06-4B71-4BA6-A14A-C0549C209E73}">
-          <x14:formula1>
-            <xm:f>ThongTinBang!$K$2:$K$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>O2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" xr:uid="{5D895D47-E29B-4177-82E0-EB6A02E4D56E}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" xr:uid="{14C06EE2-8749-4A8B-9F6C-31202F31E4F0}">
           <x14:formula1>
             <xm:f>ThongTinBang!$B$2:$B$7</xm:f>
           </x14:formula1>
           <xm:sqref>D2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" xr:uid="{AF9326B1-AFF1-4A75-B0E4-A1C74D86087D}">
+        <x14:dataValidation type="list" xr:uid="{6E02E518-2E89-4EA8-A696-E871DD0F8717}">
           <x14:formula1>
             <xm:f>ThongTinBang!$E$2:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>E2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" xr:uid="{AAFF671E-CD16-4AA6-8A0A-542406A2A2A1}">
+        <x14:dataValidation type="list" xr:uid="{A276B030-8018-4851-9183-E3292210B779}">
           <x14:formula1>
             <xm:f>ThongTinBang!$H$2:$H$3</xm:f>
           </x14:formula1>
@@ -712,11 +705,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -726,11 +717,9 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="56" customWidth="1"/>
-    <col min="11" max="11" width="103.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -749,110 +738,85 @@
       <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="K3" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>33</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>